<commit_message>
Markdown and HTML Markdown
</commit_message>
<xml_diff>
--- a/Keyword_Results.xlsx
+++ b/Keyword_Results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="274">
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -461,7 +461,7 @@
     <t xml:space="preserve">https://www.manpower.ch/de</t>
   </si>
   <si>
-    <t xml:space="preserve">}","params":{},"fields":{"mandatoryConsentText":{"value":""},"</t>
+    <t xml:space="preserve">":{"value":""},"mandatoryConsentText":{"value":""},"</t>
   </si>
   <si>
     <t xml:space="preserve">-895c-46d73197b61f","name":"Assessments and trainings","displayName</t>
@@ -485,7 +485,7 @@
     <t xml:space="preserve">":"Jobofferten Fest- und Temporärstellen | Bewerbungsunterlagen</t>
   </si>
   <si>
-    <t xml:space="preserve">value":""},"title":{"value":"Temporäreinsätze"},"image":{"value</t>
+    <t xml:space="preserve">","fields":{"title":{"value":"Temporäreinsätze"},"image":{"value</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.markritter.ch/</t>
@@ -561,9 +561,6 @@
   </si>
   <si>
     <t xml:space="preserve">Personalverleih / Try &amp; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temporäre Anstellung</t>
   </si>
   <si>
     <t xml:space="preserve">https://portfolia.ch/</t>
@@ -7037,225 +7034,223 @@
     </row>
     <row r="614">
       <c r="A614" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B614" t="s">
-        <v>12</v>
-      </c>
-      <c r="C614" t="s">
-        <v>183</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C614"/>
     </row>
     <row r="615">
       <c r="A615" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B615" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C615"/>
     </row>
     <row r="616">
       <c r="A616" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B616" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C616"/>
     </row>
     <row r="617">
       <c r="A617" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B617" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C617"/>
     </row>
     <row r="618">
       <c r="A618" t="s">
+        <v>183</v>
+      </c>
+      <c r="B618" t="s">
+        <v>8</v>
+      </c>
+      <c r="C618" t="s">
         <v>184</v>
       </c>
-      <c r="B618" t="s">
-        <v>7</v>
-      </c>
-      <c r="C618"/>
     </row>
     <row r="619">
       <c r="A619" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B619" t="s">
-        <v>8</v>
-      </c>
-      <c r="C619" t="s">
-        <v>185</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C619"/>
     </row>
     <row r="620">
       <c r="A620" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B620" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C620"/>
     </row>
     <row r="621">
       <c r="A621" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B621" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C621"/>
     </row>
     <row r="622">
       <c r="A622" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B622" t="s">
-        <v>12</v>
-      </c>
-      <c r="C622"/>
+        <v>4</v>
+      </c>
+      <c r="C622" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="623">
       <c r="A623" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B623" t="s">
-        <v>4</v>
-      </c>
-      <c r="C623" t="s">
-        <v>187</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C623"/>
     </row>
     <row r="624">
       <c r="A624" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B624" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C624"/>
     </row>
     <row r="625">
       <c r="A625" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B625" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C625"/>
     </row>
     <row r="626">
       <c r="A626" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B626" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C626"/>
     </row>
     <row r="627">
       <c r="A627" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B627" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C627"/>
     </row>
     <row r="628">
       <c r="A628" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B628" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C628"/>
     </row>
     <row r="629">
       <c r="A629" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B629" t="s">
-        <v>10</v>
-      </c>
-      <c r="C629"/>
+        <v>12</v>
+      </c>
+      <c r="C629" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="630">
       <c r="A630" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B630" t="s">
-        <v>12</v>
-      </c>
-      <c r="C630" t="s">
-        <v>188</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C630"/>
     </row>
     <row r="631">
       <c r="A631" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B631" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C631"/>
     </row>
     <row r="632">
       <c r="A632" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B632" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C632"/>
     </row>
     <row r="633">
       <c r="A633" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B633" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C633"/>
     </row>
     <row r="634">
       <c r="A634" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B634" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C634"/>
     </row>
     <row r="635">
       <c r="A635" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B635" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C635"/>
     </row>
     <row r="636">
       <c r="A636" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B636" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C636"/>
     </row>
     <row r="637">
       <c r="A637" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B637" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C637"/>
     </row>
@@ -7264,72 +7259,74 @@
         <v>189</v>
       </c>
       <c r="B638" t="s">
-        <v>12</v>
-      </c>
-      <c r="C638"/>
+        <v>4</v>
+      </c>
+      <c r="C638" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="639">
       <c r="A639" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B639" t="s">
-        <v>4</v>
-      </c>
-      <c r="C639" t="s">
-        <v>191</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C639"/>
     </row>
     <row r="640">
       <c r="A640" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B640" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C640"/>
     </row>
     <row r="641">
       <c r="A641" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B641" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C641"/>
     </row>
     <row r="642">
       <c r="A642" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B642" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C642"/>
     </row>
     <row r="643">
       <c r="A643" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B643" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C643"/>
     </row>
     <row r="644">
       <c r="A644" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B644" t="s">
-        <v>9</v>
-      </c>
-      <c r="C644"/>
+        <v>10</v>
+      </c>
+      <c r="C644" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="645">
       <c r="A645" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B645" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C645" t="s">
         <v>192</v>
@@ -7337,75 +7334,73 @@
     </row>
     <row r="646">
       <c r="A646" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B646" t="s">
-        <v>12</v>
-      </c>
-      <c r="C646" t="s">
-        <v>193</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C646"/>
     </row>
     <row r="647">
       <c r="A647" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B647" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C647"/>
     </row>
     <row r="648">
       <c r="A648" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B648" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C648"/>
     </row>
     <row r="649">
       <c r="A649" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B649" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C649"/>
     </row>
     <row r="650">
       <c r="A650" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B650" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C650"/>
     </row>
     <row r="651">
       <c r="A651" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B651" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C651"/>
     </row>
     <row r="652">
       <c r="A652" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B652" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C652"/>
     </row>
     <row r="653">
       <c r="A653" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B653" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C653"/>
     </row>
@@ -7414,49 +7409,51 @@
         <v>194</v>
       </c>
       <c r="B654" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C654"/>
     </row>
     <row r="655">
       <c r="A655" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B655" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C655"/>
     </row>
     <row r="656">
       <c r="A656" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B656" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C656"/>
     </row>
     <row r="657">
       <c r="A657" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B657" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C657"/>
     </row>
     <row r="658">
       <c r="A658" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B658" t="s">
-        <v>7</v>
-      </c>
-      <c r="C658"/>
+        <v>8</v>
+      </c>
+      <c r="C658" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="659">
       <c r="A659" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B659" t="s">
         <v>8</v>
@@ -7467,113 +7464,111 @@
     </row>
     <row r="660">
       <c r="A660" t="s">
+        <v>194</v>
+      </c>
+      <c r="B660" t="s">
+        <v>8</v>
+      </c>
+      <c r="C660" t="s">
         <v>195</v>
-      </c>
-      <c r="B660" t="s">
-        <v>8</v>
-      </c>
-      <c r="C660" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="661">
       <c r="A661" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B661" t="s">
-        <v>8</v>
-      </c>
-      <c r="C661" t="s">
-        <v>196</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C661"/>
     </row>
     <row r="662">
       <c r="A662" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B662" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C662"/>
     </row>
     <row r="663">
       <c r="A663" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B663" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C663"/>
     </row>
     <row r="664">
       <c r="A664" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B664" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C664"/>
     </row>
     <row r="665">
       <c r="A665" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B665" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C665"/>
     </row>
     <row r="666">
       <c r="A666" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B666" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C666"/>
     </row>
     <row r="667">
       <c r="A667" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B667" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C667"/>
     </row>
     <row r="668">
       <c r="A668" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B668" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C668"/>
     </row>
     <row r="669">
       <c r="A669" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B669" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C669"/>
     </row>
     <row r="670">
       <c r="A670" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B670" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C670"/>
     </row>
     <row r="671">
       <c r="A671" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B671" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C671"/>
     </row>
@@ -7582,70 +7577,70 @@
         <v>197</v>
       </c>
       <c r="B672" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C672"/>
     </row>
     <row r="673">
       <c r="A673" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B673" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C673"/>
     </row>
     <row r="674">
       <c r="A674" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B674" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C674"/>
     </row>
     <row r="675">
       <c r="A675" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B675" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C675"/>
     </row>
     <row r="676">
       <c r="A676" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B676" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C676"/>
     </row>
     <row r="677">
       <c r="A677" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B677" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C677"/>
     </row>
     <row r="678">
       <c r="A678" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B678" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C678"/>
     </row>
     <row r="679">
       <c r="A679" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B679" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C679"/>
     </row>
@@ -7654,49 +7649,51 @@
         <v>198</v>
       </c>
       <c r="B680" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C680"/>
     </row>
     <row r="681">
       <c r="A681" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B681" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C681"/>
     </row>
     <row r="682">
       <c r="A682" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B682" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C682"/>
     </row>
     <row r="683">
       <c r="A683" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B683" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C683"/>
     </row>
     <row r="684">
       <c r="A684" t="s">
+        <v>198</v>
+      </c>
+      <c r="B684" t="s">
+        <v>8</v>
+      </c>
+      <c r="C684" t="s">
         <v>199</v>
       </c>
-      <c r="B684" t="s">
-        <v>7</v>
-      </c>
-      <c r="C684"/>
     </row>
     <row r="685">
       <c r="A685" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B685" t="s">
         <v>8</v>
@@ -7707,72 +7704,72 @@
     </row>
     <row r="686">
       <c r="A686" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B686" t="s">
-        <v>8</v>
-      </c>
-      <c r="C686" t="s">
-        <v>201</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C686"/>
     </row>
     <row r="687">
       <c r="A687" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B687" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C687"/>
     </row>
     <row r="688">
       <c r="A688" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B688" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C688"/>
     </row>
     <row r="689">
       <c r="A689" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B689" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C689"/>
     </row>
     <row r="690">
       <c r="A690" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B690" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C690"/>
     </row>
     <row r="691">
       <c r="A691" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B691" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C691"/>
     </row>
     <row r="692">
       <c r="A692" t="s">
+        <v>201</v>
+      </c>
+      <c r="B692" t="s">
+        <v>7</v>
+      </c>
+      <c r="C692" t="s">
         <v>202</v>
       </c>
-      <c r="B692" t="s">
-        <v>6</v>
-      </c>
-      <c r="C692"/>
     </row>
     <row r="693">
       <c r="A693" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B693" t="s">
         <v>7</v>
@@ -7783,7 +7780,7 @@
     </row>
     <row r="694">
       <c r="A694" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B694" t="s">
         <v>7</v>
@@ -7794,92 +7791,92 @@
     </row>
     <row r="695">
       <c r="A695" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B695" t="s">
-        <v>7</v>
-      </c>
-      <c r="C695" t="s">
-        <v>205</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C695"/>
     </row>
     <row r="696">
       <c r="A696" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B696" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C696"/>
     </row>
     <row r="697">
       <c r="A697" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B697" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C697"/>
     </row>
     <row r="698">
       <c r="A698" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B698" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C698"/>
     </row>
     <row r="699">
       <c r="A699" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B699" t="s">
-        <v>12</v>
-      </c>
-      <c r="C699"/>
+        <v>4</v>
+      </c>
+      <c r="C699" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="700">
       <c r="A700" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B700" t="s">
-        <v>4</v>
-      </c>
-      <c r="C700" t="s">
-        <v>207</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C700"/>
     </row>
     <row r="701">
       <c r="A701" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B701" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C701"/>
     </row>
     <row r="702">
       <c r="A702" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B702" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C702"/>
     </row>
     <row r="703">
       <c r="A703" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B703" t="s">
-        <v>7</v>
-      </c>
-      <c r="C703"/>
+        <v>8</v>
+      </c>
+      <c r="C703" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="704">
       <c r="A704" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B704" t="s">
         <v>8</v>
@@ -7890,176 +7887,174 @@
     </row>
     <row r="705">
       <c r="A705" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B705" t="s">
-        <v>8</v>
-      </c>
-      <c r="C705" t="s">
-        <v>209</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C705"/>
     </row>
     <row r="706">
       <c r="A706" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B706" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C706"/>
     </row>
     <row r="707">
       <c r="A707" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B707" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C707"/>
     </row>
     <row r="708">
       <c r="A708" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B708" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C708"/>
     </row>
     <row r="709">
       <c r="A709" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B709" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C709"/>
     </row>
     <row r="710">
       <c r="A710" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B710" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C710"/>
     </row>
     <row r="711">
       <c r="A711" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B711" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C711"/>
     </row>
     <row r="712">
       <c r="A712" t="s">
+        <v>209</v>
+      </c>
+      <c r="B712" t="s">
+        <v>8</v>
+      </c>
+      <c r="C712" t="s">
         <v>210</v>
       </c>
-      <c r="B712" t="s">
-        <v>7</v>
-      </c>
-      <c r="C712"/>
     </row>
     <row r="713">
       <c r="A713" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B713" t="s">
-        <v>8</v>
-      </c>
-      <c r="C713" t="s">
-        <v>211</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C713"/>
     </row>
     <row r="714">
       <c r="A714" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B714" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C714"/>
     </row>
     <row r="715">
       <c r="A715" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B715" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C715"/>
     </row>
     <row r="716">
       <c r="A716" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B716" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C716"/>
     </row>
     <row r="717">
       <c r="A717" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B717" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C717"/>
     </row>
     <row r="718">
       <c r="A718" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B718" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C718"/>
     </row>
     <row r="719">
       <c r="A719" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B719" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C719"/>
     </row>
     <row r="720">
       <c r="A720" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B720" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C720"/>
     </row>
     <row r="721">
       <c r="A721" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B721" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C721"/>
     </row>
     <row r="722">
       <c r="A722" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B722" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C722"/>
     </row>
     <row r="723">
       <c r="A723" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B723" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C723"/>
     </row>
@@ -8068,67 +8063,69 @@
         <v>212</v>
       </c>
       <c r="B724" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C724"/>
     </row>
     <row r="725">
       <c r="A725" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B725" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C725"/>
     </row>
     <row r="726">
       <c r="A726" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B726" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C726"/>
     </row>
     <row r="727">
       <c r="A727" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B727" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C727"/>
     </row>
     <row r="728">
       <c r="A728" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B728" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C728"/>
     </row>
     <row r="729">
       <c r="A729" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B729" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C729"/>
     </row>
     <row r="730">
       <c r="A730" t="s">
+        <v>212</v>
+      </c>
+      <c r="B730" t="s">
+        <v>10</v>
+      </c>
+      <c r="C730" t="s">
         <v>213</v>
       </c>
-      <c r="B730" t="s">
-        <v>9</v>
-      </c>
-      <c r="C730"/>
     </row>
     <row r="731">
       <c r="A731" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B731" t="s">
         <v>10</v>
@@ -8139,10 +8136,10 @@
     </row>
     <row r="732">
       <c r="A732" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B732" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C732" t="s">
         <v>215</v>
@@ -8150,7 +8147,7 @@
     </row>
     <row r="733">
       <c r="A733" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B733" t="s">
         <v>12</v>
@@ -8161,7 +8158,7 @@
     </row>
     <row r="734">
       <c r="A734" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B734" t="s">
         <v>12</v>
@@ -8172,7 +8169,7 @@
     </row>
     <row r="735">
       <c r="A735" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B735" t="s">
         <v>12</v>
@@ -8183,7 +8180,7 @@
     </row>
     <row r="736">
       <c r="A736" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B736" t="s">
         <v>12</v>
@@ -8194,7 +8191,7 @@
     </row>
     <row r="737">
       <c r="A737" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B737" t="s">
         <v>12</v>
@@ -8205,156 +8202,154 @@
     </row>
     <row r="738">
       <c r="A738" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B738" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C738" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="739">
       <c r="A739" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B739" t="s">
-        <v>4</v>
-      </c>
-      <c r="C739" t="s">
-        <v>223</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C739"/>
     </row>
     <row r="740">
       <c r="A740" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B740" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C740"/>
     </row>
     <row r="741">
       <c r="A741" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B741" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C741"/>
     </row>
     <row r="742">
       <c r="A742" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B742" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C742"/>
     </row>
     <row r="743">
       <c r="A743" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B743" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C743"/>
     </row>
     <row r="744">
       <c r="A744" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B744" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C744"/>
     </row>
     <row r="745">
       <c r="A745" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B745" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C745"/>
     </row>
     <row r="746">
       <c r="A746" t="s">
-        <v>222</v>
-      </c>
-      <c r="B746" t="s">
-        <v>12</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B746"/>
       <c r="C746"/>
     </row>
     <row r="747">
       <c r="A747" t="s">
         <v>224</v>
       </c>
-      <c r="B747"/>
+      <c r="B747" t="s">
+        <v>4</v>
+      </c>
       <c r="C747"/>
     </row>
     <row r="748">
       <c r="A748" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B748" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C748"/>
     </row>
     <row r="749">
       <c r="A749" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B749" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C749"/>
     </row>
     <row r="750">
       <c r="A750" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B750" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C750"/>
     </row>
     <row r="751">
       <c r="A751" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B751" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C751"/>
     </row>
     <row r="752">
       <c r="A752" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B752" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C752"/>
     </row>
     <row r="753">
       <c r="A753" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B753" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C753"/>
     </row>
     <row r="754">
       <c r="A754" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B754" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C754"/>
     </row>
@@ -8363,13 +8358,15 @@
         <v>225</v>
       </c>
       <c r="B755" t="s">
-        <v>12</v>
-      </c>
-      <c r="C755"/>
+        <v>4</v>
+      </c>
+      <c r="C755" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="756">
       <c r="A756" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B756" t="s">
         <v>4</v>
@@ -8380,45 +8377,45 @@
     </row>
     <row r="757">
       <c r="A757" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B757" t="s">
-        <v>4</v>
-      </c>
-      <c r="C757" t="s">
-        <v>228</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C757"/>
     </row>
     <row r="758">
       <c r="A758" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B758" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C758"/>
     </row>
     <row r="759">
       <c r="A759" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B759" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C759"/>
     </row>
     <row r="760">
       <c r="A760" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B760" t="s">
-        <v>7</v>
-      </c>
-      <c r="C760"/>
+        <v>8</v>
+      </c>
+      <c r="C760" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="761">
       <c r="A761" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B761" t="s">
         <v>8</v>
@@ -8429,36 +8426,36 @@
     </row>
     <row r="762">
       <c r="A762" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B762" t="s">
-        <v>8</v>
-      </c>
-      <c r="C762" t="s">
-        <v>230</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C762"/>
     </row>
     <row r="763">
       <c r="A763" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B763" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C763"/>
     </row>
     <row r="764">
       <c r="A764" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B764" t="s">
-        <v>10</v>
-      </c>
-      <c r="C764"/>
+        <v>12</v>
+      </c>
+      <c r="C764" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="765">
       <c r="A765" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B765" t="s">
         <v>12</v>
@@ -8469,54 +8466,54 @@
     </row>
     <row r="766">
       <c r="A766" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B766" t="s">
-        <v>12</v>
-      </c>
-      <c r="C766" t="s">
-        <v>232</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C766"/>
     </row>
     <row r="767">
       <c r="A767" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B767" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C767"/>
     </row>
     <row r="768">
       <c r="A768" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B768" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C768"/>
     </row>
     <row r="769">
       <c r="A769" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B769" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C769"/>
     </row>
     <row r="770">
       <c r="A770" t="s">
+        <v>232</v>
+      </c>
+      <c r="B770" t="s">
+        <v>8</v>
+      </c>
+      <c r="C770" t="s">
         <v>233</v>
       </c>
-      <c r="B770" t="s">
-        <v>7</v>
-      </c>
-      <c r="C770"/>
     </row>
     <row r="771">
       <c r="A771" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B771" t="s">
         <v>8</v>
@@ -8527,94 +8524,94 @@
     </row>
     <row r="772">
       <c r="A772" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B772" t="s">
-        <v>8</v>
-      </c>
-      <c r="C772" t="s">
-        <v>235</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C772"/>
     </row>
     <row r="773">
       <c r="A773" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B773" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C773"/>
     </row>
     <row r="774">
       <c r="A774" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B774" t="s">
-        <v>10</v>
-      </c>
-      <c r="C774"/>
+        <v>12</v>
+      </c>
+      <c r="C774" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="775">
       <c r="A775" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B775" t="s">
-        <v>12</v>
-      </c>
-      <c r="C775" t="s">
-        <v>236</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C775"/>
     </row>
     <row r="776">
       <c r="A776" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B776" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C776"/>
     </row>
     <row r="777">
       <c r="A777" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B777" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C777"/>
     </row>
     <row r="778">
       <c r="A778" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B778" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C778"/>
     </row>
     <row r="779">
       <c r="A779" t="s">
+        <v>236</v>
+      </c>
+      <c r="B779" t="s">
+        <v>8</v>
+      </c>
+      <c r="C779" t="s">
         <v>237</v>
       </c>
-      <c r="B779" t="s">
-        <v>7</v>
-      </c>
-      <c r="C779"/>
     </row>
     <row r="780">
       <c r="A780" t="s">
+        <v>236</v>
+      </c>
+      <c r="B780" t="s">
+        <v>8</v>
+      </c>
+      <c r="C780" t="s">
         <v>237</v>
-      </c>
-      <c r="B780" t="s">
-        <v>8</v>
-      </c>
-      <c r="C780" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="781">
       <c r="A781" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B781" t="s">
         <v>8</v>
@@ -8625,7 +8622,7 @@
     </row>
     <row r="782">
       <c r="A782" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B782" t="s">
         <v>8</v>
@@ -8636,7 +8633,7 @@
     </row>
     <row r="783">
       <c r="A783" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B783" t="s">
         <v>8</v>
@@ -8647,10 +8644,10 @@
     </row>
     <row r="784">
       <c r="A784" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B784" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C784" t="s">
         <v>241</v>
@@ -8658,7 +8655,7 @@
     </row>
     <row r="785">
       <c r="A785" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B785" t="s">
         <v>9</v>
@@ -8669,7 +8666,7 @@
     </row>
     <row r="786">
       <c r="A786" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B786" t="s">
         <v>9</v>
@@ -8680,7 +8677,7 @@
     </row>
     <row r="787">
       <c r="A787" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B787" t="s">
         <v>9</v>
@@ -8691,7 +8688,7 @@
     </row>
     <row r="788">
       <c r="A788" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B788" t="s">
         <v>9</v>
@@ -8702,93 +8699,91 @@
     </row>
     <row r="789">
       <c r="A789" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B789" t="s">
-        <v>9</v>
-      </c>
-      <c r="C789" t="s">
-        <v>246</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C789"/>
     </row>
     <row r="790">
       <c r="A790" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B790" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C790"/>
     </row>
     <row r="791">
       <c r="A791" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B791" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C791"/>
     </row>
     <row r="792">
       <c r="A792" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B792" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C792"/>
     </row>
     <row r="793">
       <c r="A793" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B793" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C793"/>
     </row>
     <row r="794">
       <c r="A794" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B794" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C794"/>
     </row>
     <row r="795">
       <c r="A795" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B795" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C795"/>
     </row>
     <row r="796">
       <c r="A796" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B796" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C796"/>
     </row>
     <row r="797">
       <c r="A797" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B797" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C797"/>
     </row>
     <row r="798">
       <c r="A798" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B798" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C798"/>
     </row>
@@ -8797,70 +8792,70 @@
         <v>247</v>
       </c>
       <c r="B799" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C799"/>
     </row>
     <row r="800">
       <c r="A800" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B800" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C800"/>
     </row>
     <row r="801">
       <c r="A801" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B801" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C801"/>
     </row>
     <row r="802">
       <c r="A802" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B802" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C802"/>
     </row>
     <row r="803">
       <c r="A803" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B803" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C803"/>
     </row>
     <row r="804">
       <c r="A804" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B804" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C804"/>
     </row>
     <row r="805">
       <c r="A805" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B805" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C805"/>
     </row>
     <row r="806">
       <c r="A806" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B806" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C806"/>
     </row>
@@ -8869,76 +8864,78 @@
         <v>248</v>
       </c>
       <c r="B807" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C807"/>
     </row>
     <row r="808">
       <c r="A808" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B808" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C808"/>
     </row>
     <row r="809">
       <c r="A809" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B809" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C809"/>
     </row>
     <row r="810">
       <c r="A810" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B810" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C810"/>
     </row>
     <row r="811">
       <c r="A811" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B811" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C811"/>
     </row>
     <row r="812">
       <c r="A812" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B812" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C812"/>
     </row>
     <row r="813">
       <c r="A813" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B813" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C813"/>
     </row>
     <row r="814">
       <c r="A814" t="s">
+        <v>248</v>
+      </c>
+      <c r="B814" t="s">
+        <v>12</v>
+      </c>
+      <c r="C814" t="s">
         <v>249</v>
       </c>
-      <c r="B814" t="s">
-        <v>10</v>
-      </c>
-      <c r="C814"/>
     </row>
     <row r="815">
       <c r="A815" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B815" t="s">
         <v>12</v>
@@ -8949,7 +8946,7 @@
     </row>
     <row r="816">
       <c r="A816" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B816" t="s">
         <v>12</v>
@@ -8960,7 +8957,7 @@
     </row>
     <row r="817">
       <c r="A817" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B817" t="s">
         <v>12</v>
@@ -8971,7 +8968,7 @@
     </row>
     <row r="818">
       <c r="A818" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B818" t="s">
         <v>12</v>
@@ -8982,7 +8979,7 @@
     </row>
     <row r="819">
       <c r="A819" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B819" t="s">
         <v>12</v>
@@ -8993,7 +8990,7 @@
     </row>
     <row r="820">
       <c r="A820" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B820" t="s">
         <v>12</v>
@@ -9004,65 +9001,65 @@
     </row>
     <row r="821">
       <c r="A821" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B821" t="s">
         <v>12</v>
       </c>
       <c r="C821" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="822">
       <c r="A822" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B822" t="s">
-        <v>12</v>
-      </c>
-      <c r="C822" t="s">
-        <v>256</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C822"/>
     </row>
     <row r="823">
       <c r="A823" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B823" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C823"/>
     </row>
     <row r="824">
       <c r="A824" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B824" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C824"/>
     </row>
     <row r="825">
       <c r="A825" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B825" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C825"/>
     </row>
     <row r="826">
       <c r="A826" t="s">
+        <v>256</v>
+      </c>
+      <c r="B826" t="s">
+        <v>8</v>
+      </c>
+      <c r="C826" t="s">
         <v>257</v>
       </c>
-      <c r="B826" t="s">
-        <v>7</v>
-      </c>
-      <c r="C826"/>
     </row>
     <row r="827">
       <c r="A827" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B827" t="s">
         <v>8</v>
@@ -9073,102 +9070,100 @@
     </row>
     <row r="828">
       <c r="A828" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B828" t="s">
-        <v>8</v>
-      </c>
-      <c r="C828" t="s">
-        <v>259</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C828"/>
     </row>
     <row r="829">
       <c r="A829" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B829" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C829"/>
     </row>
     <row r="830">
       <c r="A830" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B830" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C830"/>
     </row>
     <row r="831">
       <c r="A831" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B831" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C831"/>
     </row>
     <row r="832">
       <c r="A832" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B832" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C832"/>
     </row>
     <row r="833">
       <c r="A833" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B833" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C833"/>
     </row>
     <row r="834">
       <c r="A834" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B834" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C834"/>
     </row>
     <row r="835">
       <c r="A835" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B835" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C835"/>
     </row>
     <row r="836">
       <c r="A836" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B836" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C836"/>
     </row>
     <row r="837">
       <c r="A837" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B837" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C837"/>
     </row>
     <row r="838">
       <c r="A838" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B838" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C838"/>
     </row>
@@ -9177,80 +9172,82 @@
         <v>260</v>
       </c>
       <c r="B839" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C839"/>
     </row>
     <row r="840">
       <c r="A840" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B840" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C840"/>
     </row>
     <row r="841">
       <c r="A841" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B841" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C841"/>
     </row>
     <row r="842">
       <c r="A842" t="s">
+        <v>260</v>
+      </c>
+      <c r="B842" t="s">
+        <v>7</v>
+      </c>
+      <c r="C842" t="s">
         <v>261</v>
       </c>
-      <c r="B842" t="s">
-        <v>6</v>
-      </c>
-      <c r="C842"/>
     </row>
     <row r="843">
       <c r="A843" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B843" t="s">
-        <v>7</v>
-      </c>
-      <c r="C843" t="s">
-        <v>262</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C843"/>
     </row>
     <row r="844">
       <c r="A844" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B844" t="s">
-        <v>8</v>
-      </c>
-      <c r="C844"/>
+        <v>9</v>
+      </c>
+      <c r="C844" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="845">
       <c r="A845" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B845" t="s">
-        <v>9</v>
-      </c>
-      <c r="C845" t="s">
-        <v>263</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C845"/>
     </row>
     <row r="846">
       <c r="A846" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B846" t="s">
-        <v>10</v>
-      </c>
-      <c r="C846"/>
+        <v>12</v>
+      </c>
+      <c r="C846" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="847">
       <c r="A847" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B847" t="s">
         <v>12</v>
@@ -9261,7 +9258,7 @@
     </row>
     <row r="848">
       <c r="A848" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B848" t="s">
         <v>12</v>
@@ -9272,7 +9269,7 @@
     </row>
     <row r="849">
       <c r="A849" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B849" t="s">
         <v>12</v>
@@ -9283,7 +9280,7 @@
     </row>
     <row r="850">
       <c r="A850" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B850" t="s">
         <v>12</v>
@@ -9294,7 +9291,7 @@
     </row>
     <row r="851">
       <c r="A851" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B851" t="s">
         <v>12</v>
@@ -9305,7 +9302,7 @@
     </row>
     <row r="852">
       <c r="A852" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B852" t="s">
         <v>12</v>
@@ -9316,7 +9313,7 @@
     </row>
     <row r="853">
       <c r="A853" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B853" t="s">
         <v>12</v>
@@ -9327,7 +9324,7 @@
     </row>
     <row r="854">
       <c r="A854" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B854" t="s">
         <v>12</v>
@@ -9338,7 +9335,7 @@
     </row>
     <row r="855">
       <c r="A855" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B855" t="s">
         <v>12</v>
@@ -9349,81 +9346,81 @@
     </row>
     <row r="856">
       <c r="A856" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B856" t="s">
-        <v>12</v>
-      </c>
-      <c r="C856" t="s">
-        <v>273</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C856"/>
     </row>
     <row r="857">
       <c r="A857" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B857" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C857"/>
     </row>
     <row r="858">
       <c r="A858" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B858" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C858"/>
     </row>
     <row r="859">
       <c r="A859" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B859" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C859"/>
     </row>
     <row r="860">
       <c r="A860" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B860" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C860"/>
     </row>
     <row r="861">
       <c r="A861" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B861" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C861"/>
     </row>
     <row r="862">
       <c r="A862" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B862" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C862"/>
     </row>
     <row r="863">
       <c r="A863" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B863" t="s">
-        <v>10</v>
-      </c>
-      <c r="C863"/>
+        <v>12</v>
+      </c>
+      <c r="C863" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="864">
       <c r="A864" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B864" t="s">
         <v>12</v>
@@ -9434,7 +9431,7 @@
     </row>
     <row r="865">
       <c r="A865" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B865" t="s">
         <v>12</v>
@@ -9445,7 +9442,7 @@
     </row>
     <row r="866">
       <c r="A866" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B866" t="s">
         <v>12</v>
@@ -9456,34 +9453,12 @@
     </row>
     <row r="867">
       <c r="A867" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B867" t="s">
         <v>12</v>
       </c>
       <c r="C867" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="868">
-      <c r="A868" t="s">
-        <v>274</v>
-      </c>
-      <c r="B868" t="s">
-        <v>12</v>
-      </c>
-      <c r="C868" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="869">
-      <c r="A869" t="s">
-        <v>274</v>
-      </c>
-      <c r="B869" t="s">
-        <v>12</v>
-      </c>
-      <c r="C869" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>